<commit_message>
Extend Login\Register negative test cases
</commit_message>
<xml_diff>
--- a/Test Cases/Negative Test Cases/Log in Test Suite.xlsx
+++ b/Test Cases/Negative Test Cases/Log in Test Suite.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="38">
   <si>
     <t>Test Case № 1</t>
   </si>
@@ -59,6 +59,75 @@
   </si>
   <si>
     <t>"Email and/or password don’t match"error appears</t>
+  </si>
+  <si>
+    <t>Test Case № 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to log in with empty Email filed and correct password </t>
+  </si>
+  <si>
+    <t>2. Leave the Email adress field empty.</t>
+  </si>
+  <si>
+    <t>3. In the Password field write valid user password "test"</t>
+  </si>
+  <si>
+    <t>Test Case № 4</t>
+  </si>
+  <si>
+    <t>2. In the Email adress field write invalid  Email : "a@ccom"</t>
+  </si>
+  <si>
+    <t>Test Case № 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to log in with too long Email and correct password </t>
+  </si>
+  <si>
+    <t>2. In the Email adress field write valid Email string which length are &gt; 64 chars</t>
+  </si>
+  <si>
+    <t>Test Case № 6</t>
+  </si>
+  <si>
+    <t>Try to log in with empty password field and correct Email</t>
+  </si>
+  <si>
+    <t>2. In the Email adress field write "test@gmail.com"</t>
+  </si>
+  <si>
+    <t>3. Leave the Password field empty</t>
+  </si>
+  <si>
+    <t>Test Case № 7</t>
+  </si>
+  <si>
+    <t>3. In the Password field write "tst"</t>
+  </si>
+  <si>
+    <t>3. In the Password field write "test"</t>
+  </si>
+  <si>
+    <t>Test Case № 8</t>
+  </si>
+  <si>
+    <t>Try to log in with too long password and correct Email field</t>
+  </si>
+  <si>
+    <t>3. In the Password field write string which length are &gt; 64 chars</t>
+  </si>
+  <si>
+    <t>Try to log in with short password (&lt; 4 chars) and correct Email field</t>
+  </si>
+  <si>
+    <t>"Incorrect Length for Email"error appears</t>
+  </si>
+  <si>
+    <t>"Email is not a valid email address"error appears</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to log in with invalid Email and correct password </t>
   </si>
 </sst>
 </file>
@@ -74,15 +143,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -90,12 +165,157 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -156,7 +376,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -191,7 +411,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -400,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,104 +635,462 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>6</v>
       </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="10" t="s">
         <v>10</v>
       </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
+      <c r="C11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="C12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6"/>
+      <c r="B31" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6"/>
+      <c r="B37" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="5"/>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="6"/>
+      <c r="B49" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>